<commit_message>
Corousal fixes and uodated unit test document
</commit_message>
<xml_diff>
--- a/UnitTestDoc.xlsx
+++ b/UnitTestDoc.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anuragsengupta/Desktop/CS-297P/GamersHub/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{04E6A1D3-0316-5148-8A85-E1E35394F7F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{248DF304-9E4E-6849-AC00-4BA0FFF2A692}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{1423AE88-5CF6-E949-8068-D66325D5155B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$24</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="28">
   <si>
     <t>Description</t>
   </si>
@@ -57,9 +60,6 @@
     <t>When the user clicks on Login in the register page, it should redirect the user to the login page</t>
   </si>
   <si>
-    <t>In Progress</t>
-  </si>
-  <si>
     <t>An already registered user shouldn't be allowed to register again</t>
   </si>
   <si>
@@ -82,6 +82,45 @@
   </si>
   <si>
     <t>The endpoint APIs for both login and register should work and validate the business rules</t>
+  </si>
+  <si>
+    <t>Home page top games, latest game redirection</t>
+  </si>
+  <si>
+    <t>Twitch scroll view playing video with the metadata and close button</t>
+  </si>
+  <si>
+    <t>Logout button dropdown is working across all screens</t>
+  </si>
+  <si>
+    <t>Navigation bar buttons are working</t>
+  </si>
+  <si>
+    <t>Able to logout from all the screen</t>
+  </si>
+  <si>
+    <t>Steam screen login page load but close without authentication, crashes the screen</t>
+  </si>
+  <si>
+    <t>Recommendations within steam page</t>
+  </si>
+  <si>
+    <t>Redirection URLs working</t>
+  </si>
+  <si>
+    <t>Twitch authentication</t>
+  </si>
+  <si>
+    <t>Twitch past and live streams</t>
+  </si>
+  <si>
+    <t>Support page, entry</t>
+  </si>
+  <si>
+    <t>Support page submit</t>
+  </si>
+  <si>
+    <t>Recommendations within EPIC page</t>
   </si>
 </sst>
 </file>
@@ -105,7 +144,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -121,12 +160,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -174,9 +207,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -497,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D449C7AA-6381-BA49-9EA0-C70BF53140BA}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -521,7 +556,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="6">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -532,7 +567,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="6">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -543,94 +578,238 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="6">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="6">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C6" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="B8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" s="5">
         <v>9</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="6">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="B10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="5">
         <v>10</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="6">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="5">
         <v>11</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="B12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="5">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="6">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="B13" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="5">
         <v>13</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="6">
-        <v>9</v>
-      </c>
-      <c r="B10" s="2" t="s">
+      <c r="B14" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="5">
         <v>14</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A11" s="6">
-        <v>10</v>
-      </c>
-      <c r="B11" s="2" t="s">
+      <c r="B15" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="5">
         <v>15</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>4</v>
+      <c r="B16" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="5">
+        <v>16</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="5">
+        <v>17</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="5">
+        <v>18</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="5">
+        <v>19</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="5">
+        <v>20</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="5">
+        <v>21</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="5">
+        <v>22</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="5">
+        <v>23</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C24" xr:uid="{57932146-13C0-BE49-AB7D-3FB174023136}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>